<commit_message>
hotfix: Fix AccessPoint parameters for Add/Del Obj
Signed-off-by: Vladyslav Tupikin <v.tupikin@inango-systems.com>
</commit_message>
<xml_diff>
--- a/customers/inango-prplmesh-en/model/prplmesh-generator.xlsx
+++ b/customers/inango-prplmesh-en/model/prplmesh-generator.xlsx
@@ -385,10 +385,10 @@
     <t xml:space="preserve">prplmesh_set.lua Controller.Network.AccessPoint.$$;AccessPointIndex</t>
   </si>
   <si>
-    <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint.{i}; ; idx = AccessPointIndex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prplmesh_del.lua Device.Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
+    <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prplmesh_del.lua Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
   </si>
   <si>
     <t xml:space="preserve">prplmesh_getall.lua Controller.Network.AccessPoint.{i}; idx = AccessPointIndex</t>
@@ -1906,8 +1906,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{DBB257D1-0287-4F11-99DF-40B2F57C9CA9}">
-  <header guid="{F5786B15-5DAB-4926-9418-9C204B64E28B}" dateTime="2021-02-16T15:27:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="7">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{AEBCA880-B033-488A-ABE0-0D3BF8B11912}">
+  <header guid="{014A4AA8-FD3C-4BAC-8114-2A59F8FA4BB7}" dateTime="2021-02-16T15:27:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1917,7 +1917,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{240C5FEC-F7BE-4024-A7D5-2700B8A07112}" dateTime="2021-02-16T17:43:00.000000000Z" userName=" " r:id="rId2" minRId="3" maxRId="4" maxSheetId="7">
+  <header guid="{69E0D0E9-7114-4521-9B21-913F50E0037C}" dateTime="2021-02-16T15:31:00.000000000Z" userName=" " r:id="rId2" minRId="3" maxRId="3" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1927,7 +1927,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{FCAFCABA-B906-4AE0-B1D4-9ACAC2109688}" dateTime="2021-02-16T17:44:00.000000000Z" userName=" " r:id="rId3" minRId="5" maxRId="8" maxSheetId="7">
+  <header guid="{971B0A7C-18DF-4007-AF21-2DFE0BFA437A}" dateTime="2021-02-16T15:32:00.000000000Z" userName=" " r:id="rId3" minRId="4" maxRId="6" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1937,7 +1937,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{85B8D7AC-3F26-4E14-B134-CD4DC338AA62}" dateTime="2021-02-16T15:39:00.000000000Z" userName=" " r:id="rId4" minRId="9" maxRId="9" maxSheetId="7">
+  <header guid="{E03ACA37-1B4E-4A08-9B95-17471833CB26}" dateTime="2021-02-16T15:38:00.000000000Z" userName=" " r:id="rId4" minRId="7" maxRId="8" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1947,7 +1947,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{3F0A7D15-F655-49F6-9148-32390629A784}" dateTime="2021-02-16T17:45:00.000000000Z" userName=" " r:id="rId5" minRId="10" maxRId="10" maxSheetId="7">
+  <header guid="{6470D23D-AEC2-469C-BB3C-9AD79530E678}" dateTime="2021-02-16T15:33:00.000000000Z" userName=" " r:id="rId5" minRId="9" maxRId="9" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1957,7 +1957,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{F4A873CC-7131-4395-8126-4132BE7D801A}" dateTime="2021-02-16T17:48:00.000000000Z" userName=" " r:id="rId6" minRId="11" maxRId="11" maxSheetId="7">
+  <header guid="{1F82C6C4-C1EC-4AFC-B63D-F555ABA4AC32}" dateTime="2021-02-16T15:35:00.000000000Z" userName=" " r:id="rId6" minRId="10" maxRId="13" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1967,7 +1967,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{FEC88481-A301-46F3-9180-56AEB1E14B1E}" dateTime="2021-02-16T17:49:00.000000000Z" userName=" " r:id="rId7" minRId="12" maxRId="12" maxSheetId="7">
+  <header guid="{086878BA-B54C-4A05-B764-7333DF3F4947}" dateTime="2021-02-16T15:37:00.000000000Z" userName=" " r:id="rId7" minRId="14" maxRId="14" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1977,7 +1977,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{88B21C42-60B1-4EAF-ACBA-AE3313BB5DB9}" dateTime="2021-02-16T15:29:00.000000000Z" userName=" " r:id="rId8" minRId="13" maxRId="13" maxSheetId="7">
+  <header guid="{5F2F1F2E-156E-4366-90BF-0FEF64F74171}" dateTime="2021-02-16T17:58:00.000000000Z" userName=" " r:id="rId8" minRId="15" maxRId="15" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1987,7 +1987,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{B4A9B712-D64F-4403-AEAB-BF644976B82A}" dateTime="2021-02-16T15:30:00.000000000Z" userName=" " r:id="rId9" minRId="14" maxRId="14" maxSheetId="7">
+  <header guid="{6793CB85-BD3D-438E-9737-3843CA8F02BB}" dateTime="2021-02-16T17:59:00.000000000Z" userName=" " r:id="rId9" minRId="16" maxRId="16" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1997,7 +1997,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{1A455510-2C83-446F-A6DF-4E9695AFF413}" dateTime="2021-02-16T15:31:00.000000000Z" userName=" " r:id="rId10" minRId="15" maxRId="15" maxSheetId="7">
+  <header guid="{864066BD-D552-498C-AB9A-BA42CCE5AB55}" dateTime="2021-02-16T18:01:00.000000000Z" userName=" " r:id="rId10" minRId="17" maxRId="17" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2007,7 +2007,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{8FE9A7C8-B71F-4668-95B0-D85F7E471146}" dateTime="2021-02-16T15:32:00.000000000Z" userName=" " r:id="rId11" minRId="16" maxRId="18" maxSheetId="7">
+  <header guid="{EA53141E-9217-4FC7-BB40-4B3514B4AB99}" dateTime="2021-02-16T18:03:00.000000000Z" userName=" " r:id="rId11" minRId="18" maxRId="19" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2017,7 +2017,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{B4BD6166-C67D-4016-9FA5-A195BC14EC06}" dateTime="2021-02-16T15:38:00.000000000Z" userName=" " r:id="rId12" minRId="19" maxRId="20" maxSheetId="7">
+  <header guid="{3B49C647-2B97-4009-B8AC-BAB194DE3E98}" dateTime="2021-02-16T17:43:00.000000000Z" userName=" " r:id="rId12" minRId="20" maxRId="21" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2027,7 +2027,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{E887A9F4-5B39-4B96-B6B9-BBF7DE48481C}" dateTime="2021-02-16T15:33:00.000000000Z" userName=" " r:id="rId13" minRId="21" maxRId="21" maxSheetId="7">
+  <header guid="{8D952353-A148-4F19-A4FA-A2C9E589729C}" dateTime="2021-02-16T18:06:00.000000000Z" userName=" " r:id="rId13" minRId="22" maxRId="23" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2037,7 +2037,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{D31725ED-ED06-4DDF-AD16-19218747541F}" dateTime="2021-02-16T15:35:00.000000000Z" userName=" " r:id="rId14" minRId="22" maxRId="25" maxSheetId="7">
+  <header guid="{8B0DF753-55BA-469C-8CCC-E1E607162C23}" dateTime="2021-02-16T17:35:00.000000000Z" userName=" " r:id="rId14" minRId="24" maxRId="25" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2047,7 +2047,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{77A6C909-C153-4485-A258-B17A3A71028D}" dateTime="2021-02-16T15:37:00.000000000Z" userName=" " r:id="rId15" minRId="26" maxRId="26" maxSheetId="7">
+  <header guid="{87A26D1E-006E-4ACE-9CF3-B4A975BD95D4}" dateTime="2021-02-16T17:36:00.000000000Z" userName=" " r:id="rId15" minRId="26" maxRId="27" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2057,7 +2057,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6BBE931F-5DEC-4F8B-AD86-BA10143F71C3}" dateTime="2021-02-16T17:58:00.000000000Z" userName=" " r:id="rId16" minRId="27" maxRId="27" maxSheetId="7">
+  <header guid="{D19E2B6C-6352-4DB9-B42B-7A7692132797}" dateTime="2021-02-16T17:37:00.000000000Z" userName=" " r:id="rId16" minRId="28" maxRId="29" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2067,7 +2067,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6976DA0C-5693-4556-A87F-CEA478A87437}" dateTime="2021-02-16T17:59:00.000000000Z" userName=" " r:id="rId17" minRId="28" maxRId="28" maxSheetId="7">
+  <header guid="{52831D17-EF36-4CD9-98B3-F55952298861}" dateTime="2021-02-16T17:38:00.000000000Z" userName=" " r:id="rId17" minRId="30" maxRId="31" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2077,7 +2077,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{39D2E541-99C3-4613-B071-053C271512F4}" dateTime="2021-02-16T18:01:00.000000000Z" userName=" " r:id="rId18" minRId="29" maxRId="29" maxSheetId="7">
+  <header guid="{308D37A9-A032-444F-A936-286BE24D7783}" dateTime="2021-02-16T17:40:00.000000000Z" userName=" " r:id="rId18" minRId="32" maxRId="32" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2087,7 +2087,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{B5E41EBC-FB22-44ED-B42E-597B0C212213}" dateTime="2021-02-16T18:03:00.000000000Z" userName=" " r:id="rId19" minRId="30" maxRId="31" maxSheetId="7">
+  <header guid="{36529D9D-847D-46B0-9F49-E5F34DA3A77A}" dateTime="2021-02-16T17:41:00.000000000Z" userName=" " r:id="rId19" minRId="33" maxRId="34" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2097,7 +2097,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{AF4BE15A-7D3D-4C61-AC92-C06B625F3F98}" dateTime="2021-02-16T18:06:00.000000000Z" userName=" " r:id="rId20" minRId="32" maxRId="33" maxSheetId="7">
+  <header guid="{4DA7347C-BAF0-4036-AB05-E3FCAE601A4B}" dateTime="2021-02-16T17:42:00.000000000Z" userName=" " r:id="rId20" minRId="35" maxRId="35" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2107,7 +2107,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{9AD4F644-4F14-4E38-A671-22AA3EA4916E}" dateTime="2021-02-16T17:35:00.000000000Z" userName=" " r:id="rId21" minRId="34" maxRId="35" maxSheetId="7">
+  <header guid="{6DDB52B4-0F7B-4DFA-B581-458C55CEA3AC}" dateTime="2021-02-16T18:12:00.000000000Z" userName=" " r:id="rId21" minRId="36" maxRId="36" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2117,7 +2117,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{76119C32-FB2D-4CE9-8C8D-AA1FAC0B6B4B}" dateTime="2021-02-16T17:36:00.000000000Z" userName=" " r:id="rId22" minRId="36" maxRId="37" maxSheetId="7">
+  <header guid="{6F908CB5-5CC2-4D31-B024-91DD3F7A2898}" dateTime="2021-02-16T18:13:00.000000000Z" userName=" " r:id="rId22" minRId="37" maxRId="37" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2127,7 +2127,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{C82F5ED9-66D6-468F-93FA-3DB75619488A}" dateTime="2021-02-16T17:37:00.000000000Z" userName=" " r:id="rId23" minRId="38" maxRId="39" maxSheetId="7">
+  <header guid="{D2B1F965-C60F-4CF9-89EE-C9A4E738DF82}" dateTime="2021-02-16T17:44:00.000000000Z" userName=" " r:id="rId23" minRId="38" maxRId="41" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2137,7 +2137,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{7BB8F3D1-B087-45E8-8DCA-2B7C1764A47E}" dateTime="2021-02-16T17:38:00.000000000Z" userName=" " r:id="rId24" minRId="40" maxRId="41" maxSheetId="7">
+  <header guid="{B5D70D94-E975-44DF-B752-2C8BA9AFCEE0}" dateTime="2021-02-16T18:14:00.000000000Z" userName=" " r:id="rId24" minRId="42" maxRId="42" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2147,7 +2147,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{FC09BACC-F39F-45E8-BC00-C0EA8A4EA448}" dateTime="2021-02-16T17:40:00.000000000Z" userName=" " r:id="rId25" minRId="42" maxRId="42" maxSheetId="7">
+  <header guid="{F6821565-9363-4F63-A9BD-E99950E500EF}" dateTime="2021-02-16T18:16:00.000000000Z" userName=" " r:id="rId25" minRId="43" maxRId="43" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2157,7 +2157,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{84A459C7-01B9-4135-AED5-C8DD2C20F523}" dateTime="2021-02-16T17:41:00.000000000Z" userName=" " r:id="rId26" minRId="43" maxRId="44" maxSheetId="7">
+  <header guid="{52A3BFEC-31FD-41EB-A5BB-4C9660575455}" dateTime="2021-02-16T15:39:00.000000000Z" userName=" " r:id="rId26" minRId="44" maxRId="44" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2167,7 +2167,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{70940909-400F-43FB-8512-E0F614129D68}" dateTime="2021-02-16T17:42:00.000000000Z" userName=" " r:id="rId27" minRId="45" maxRId="45" maxSheetId="7">
+  <header guid="{26103682-AC5E-471B-A220-C9F41262E02D}" dateTime="2021-02-16T17:45:00.000000000Z" userName=" " r:id="rId27" minRId="45" maxRId="45" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2177,7 +2177,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{177EC065-D4D6-4B90-AEA7-74052638A0C1}" dateTime="2021-02-16T18:12:00.000000000Z" userName=" " r:id="rId28" minRId="46" maxRId="46" maxSheetId="7">
+  <header guid="{83AFDAAB-9244-41BB-9A46-831166069DCE}" dateTime="2021-02-16T17:48:00.000000000Z" userName=" " r:id="rId28" minRId="46" maxRId="46" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2187,7 +2187,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{D3413631-EDF8-4046-9BC9-FBC3C4A90DFC}" dateTime="2021-02-16T18:13:00.000000000Z" userName=" " r:id="rId29" minRId="47" maxRId="47" maxSheetId="7">
+  <header guid="{6D4AE0C1-77FD-40D6-A87A-00CFF4AFB4CF}" dateTime="2021-02-16T17:49:00.000000000Z" userName=" " r:id="rId29" minRId="47" maxRId="47" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2197,7 +2197,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{CE77C04C-C5C9-4696-9FE0-E419008F0A13}" dateTime="2021-02-16T18:14:00.000000000Z" userName=" " r:id="rId30" minRId="48" maxRId="48" maxSheetId="7">
+  <header guid="{53FB02C1-6BFC-4FB7-975C-FC95FFAFFA11}" dateTime="2021-02-16T15:29:00.000000000Z" userName=" " r:id="rId30" minRId="48" maxRId="48" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2207,7 +2207,27 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{DBB257D1-0287-4F11-99DF-40B2F57C9CA9}" dateTime="2021-02-16T18:16:00.000000000Z" userName=" " r:id="rId31" minRId="49" maxRId="49" maxSheetId="7">
+  <header guid="{0FA86F92-ED6E-4610-927E-F28499665025}" dateTime="2021-02-16T15:30:00.000000000Z" userName=" " r:id="rId31" minRId="49" maxRId="49" maxSheetId="7">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B443AD7F-CFDE-4DE6-B03E-9119965C8268}" dateTime="2021-02-17T20:37:00.000000000Z" userName=" " r:id="rId32" minRId="50" maxRId="50" maxSheetId="7">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AEBCA880-B033-488A-ABE0-0D3BF8B11912}" dateTime="2021-02-17T20:38:00.000000000Z" userName=" " r:id="rId33" minRId="51" maxRId="52" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2283,7 +2303,561 @@
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="15" ua="false" sId="2">
+  <rcc rId="17" ua="false" sId="2">
+    <oc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,с</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="18" ua="false" sId="2">
+    <oc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,с</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="19" ua="false" sId="2">
+    <oc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="20" ua="false" sId="2">
+    <oc r="AL30" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = RadioIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL30" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = RadioIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" ua="false" sId="2">
+    <oc r="AL42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="22" ua="false" sId="2">
+    <oc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OperatingClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="23" ua="false" sId="2">
+    <oc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="24" ua="false" sId="2">
+    <oc r="AD30" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$;Controller.Network.Device.{i}.DeviceIndex,RadioIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD30" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$;Device.Controller.Network.Device.{i}.DeviceIndex,RadioIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="25" ua="false" sId="2">
+    <oc r="AD42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="26" ua="false" sId="2">
+    <oc r="AD47" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD47" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="27" ua="false" sId="2">
+    <oc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="28" ua="false" sId="2">
+    <oc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="29" ua="false" sId="2">
+    <oc r="AD54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="30" ua="false" sId="2">
+    <oc r="AD71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$.STA.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex,STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$.STA.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex,STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="31" ua="false" sId="2">
+    <oc r="AD94" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BackhaulSTA;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD94" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BackhaulSTA;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="32" ua="false" sId="2">
+    <oc r="AD97" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD97" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="33" ua="false" sId="2">
+    <oc r="AD99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="34" ua="false" sId="2">
+    <oc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="3" ua="false" sId="2">
     <oc r="AL42" t="inlineStr">
       <is>
         <r>
@@ -2314,9 +2888,423 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="16" ua="false" sId="2">
+  <rcc rId="35" ua="false" sId="2">
+    <oc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="36" ua="false" sId="2">
+    <oc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="37" ua="false" sId="2">
+    <oc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="38" ua="false" sId="2">
+    <oc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="39" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="40" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="41" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="42" ua="false" sId="2">
+    <oc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="43" ua="false" sId="2">
+    <oc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="44" ua="false" sId="2">
+    <oc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex, idx = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="45" ua="false" sId="2">
+    <oc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="46" ua="false" sId="2">
+    <oc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="47" ua="false" sId="2">
+    <oc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="4" ua="false" sId="2">
     <oc r="AL54" t="inlineStr">
       <is>
         <r>
@@ -2344,7 +3332,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="17" ua="false" sId="2">
+  <rcc rId="5" ua="false" sId="2">
     <oc r="AL71" t="inlineStr">
       <is>
         <r>
@@ -2372,7 +3360,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="18" ua="false" sId="2">
+  <rcc rId="6" ua="false" sId="2">
     <oc r="AL71" t="inlineStr">
       <is>
         <r>
@@ -2403,9 +3391,175 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="19" ua="false" sId="2">
+  <rcc rId="48" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.; idx = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="49" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="50" ua="false" sId="2">
+    <oc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint.{i}; ; idx = AccessPointIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; </t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="51" ua="false" sId="2">
+    <oc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; </t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="52" ua="false" sId="2">
+    <oc r="AJ10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_del.lua Device.Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AJ10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_del.lua Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="7" ua="false" sId="2">
     <oc r="AL108" t="inlineStr">
       <is>
         <r>
@@ -2433,7 +3587,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="20" ua="false" sId="2">
+  <rcc rId="8" ua="false" sId="2">
     <oc r="AL102" t="inlineStr">
       <is>
         <r>
@@ -2464,9 +3618,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="21" ua="false" sId="2">
+  <rcc rId="9" ua="false" sId="2">
     <oc r="AL71" t="inlineStr">
       <is>
         <r>
@@ -2497,9 +3651,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="22" ua="false" sId="2">
+  <rcc rId="10" ua="false" sId="2">
     <oc r="AL99" t="inlineStr">
       <is>
         <r>
@@ -2527,7 +3681,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="23" ua="false" sId="2">
+  <rcc rId="11" ua="false" sId="2">
     <oc r="AL49" t="inlineStr">
       <is>
         <r>
@@ -2555,7 +3709,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="24" ua="false" sId="2">
+  <rcc rId="12" ua="false" sId="2">
     <oc r="AL54" t="inlineStr">
       <is>
         <r>
@@ -2583,7 +3737,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="25" ua="false" sId="2">
+  <rcc rId="13" ua="false" sId="2">
     <oc r="AL99" t="inlineStr">
       <is>
         <r>
@@ -2614,9 +3768,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="26" ua="false" sId="2">
+  <rcc rId="14" ua="false" sId="2">
     <oc r="AL102" t="inlineStr">
       <is>
         <r>
@@ -2647,9 +3801,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="27" ua="false" sId="2">
+  <rcc rId="15" ua="false" sId="2">
     <oc r="AD42" t="inlineStr">
       <is>
         <r>
@@ -2680,9 +3834,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="28" ua="false" sId="2">
+  <rcc rId="16" ua="false" sId="2">
     <oc r="AL42" t="inlineStr">
       <is>
         <r>
@@ -2706,1048 +3860,6 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOperatingClassesIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="29" ua="false" sId="2">
-    <oc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,с</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="30" ua="false" sId="2">
-    <oc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,с</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="31" ua="false" sId="2">
-    <oc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="3" ua="false" sId="2">
-    <oc r="AL30" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = RadioIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL30" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = RadioIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="4" ua="false" sId="2">
-    <oc r="AL42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="32" ua="false" sId="2">
-    <oc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OperatingClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="33" ua="false" sId="2">
-    <oc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="34" ua="false" sId="2">
-    <oc r="AD30" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$;Controller.Network.Device.{i}.DeviceIndex,RadioIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD30" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$;Device.Controller.Network.Device.{i}.DeviceIndex,RadioIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="35" ua="false" sId="2">
-    <oc r="AD42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="36" ua="false" sId="2">
-    <oc r="AD47" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD47" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="37" ua="false" sId="2">
-    <oc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i};Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="38" ua="false" sId="2">
-    <oc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.{i}.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="39" ua="false" sId="2">
-    <oc r="AD54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="40" ua="false" sId="2">
-    <oc r="AD71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$.STA.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex,STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BSS.$$.STA.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex,STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="41" ua="false" sId="2">
-    <oc r="AD94" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BackhaulSTA;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD94" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.BackhaulSTA;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="42" ua="false" sId="2">
-    <oc r="AD97" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD97" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="43" ua="false" sId="2">
-    <oc r="AD99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="44" ua="false" sId="2">
-    <oc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="45" ua="false" sId="2">
-    <oc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="46" ua="false" sId="2">
-    <oc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="47" ua="false" sId="2">
-    <oc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="5" ua="false" sId="2">
-    <oc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="6" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="7" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="48" ua="false" sId="2">
-    <oc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="49" ua="false" sId="2">
-    <oc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="9" ua="false" sId="2">
-    <oc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex, idx = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="10" ua="false" sId="2">
-    <oc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="11" ua="false" sId="2">
-    <oc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="12" ua="false" sId="2">
-    <oc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="13" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.; idx = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="14" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
         </r>
       </is>
     </nc>
@@ -3868,11 +3980,11 @@
   <dimension ref="A1:AMJ115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AA1" activeCellId="0" sqref="AA1"/>
+      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD108" activeCellId="0" sqref="AD108"/>
+      <selection pane="bottomRight" activeCell="AF17" activeCellId="0" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
MMX model for prplMesh: fixed AddObjMethod for AccessPoint object
To fix error
    operation have to return anything in column AddObjMethod

Changed AddObjMethod
for Device.Controller.Network.AccessPoint.{i}.  object from

    prplmesh_add.lua Controller.Network.AccessPoint

to

    prplmesh_add.lua Controller.Network.AccessPoint; ; idx = AccessPointIndex

Signed-off-by: Ivan Efimov <i.efimov@inango-systems.com>
</commit_message>
<xml_diff>
--- a/customers/inango-prplmesh-en/model/prplmesh-generator.xlsx
+++ b/customers/inango-prplmesh-en/model/prplmesh-generator.xlsx
@@ -385,7 +385,7 @@
     <t xml:space="preserve">prplmesh_set.lua Controller.Network.AccessPoint.$$;AccessPointIndex</t>
   </si>
   <si>
-    <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint</t>
+    <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; ; idx = AccessPointIndex</t>
   </si>
   <si>
     <t xml:space="preserve">prplmesh_del.lua Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
@@ -1906,8 +1906,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{AEBCA880-B033-488A-ABE0-0D3BF8B11912}">
-  <header guid="{014A4AA8-FD3C-4BAC-8114-2A59F8FA4BB7}" dateTime="2021-02-16T15:27:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="7">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{FEEE1EC7-3F41-4468-B84C-3834F9955678}">
+  <header guid="{13246DC0-CFC2-4596-875D-690CF7DB819B}" dateTime="2021-02-16T15:27:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1917,7 +1917,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{69E0D0E9-7114-4521-9B21-913F50E0037C}" dateTime="2021-02-16T15:31:00.000000000Z" userName=" " r:id="rId2" minRId="3" maxRId="3" maxSheetId="7">
+  <header guid="{44B68D95-7765-483E-8576-9E4FF84D6EC4}" dateTime="2021-02-16T18:01:00.000000000Z" userName=" " r:id="rId2" minRId="3" maxRId="3" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1927,7 +1927,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{971B0A7C-18DF-4007-AF21-2DFE0BFA437A}" dateTime="2021-02-16T15:32:00.000000000Z" userName=" " r:id="rId3" minRId="4" maxRId="6" maxSheetId="7">
+  <header guid="{42CB9E2D-B048-4B3E-966E-7476B5244B45}" dateTime="2021-02-16T18:03:00.000000000Z" userName=" " r:id="rId3" minRId="4" maxRId="5" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1937,7 +1937,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{E03ACA37-1B4E-4A08-9B95-17471833CB26}" dateTime="2021-02-16T15:38:00.000000000Z" userName=" " r:id="rId4" minRId="7" maxRId="8" maxSheetId="7">
+  <header guid="{E85EDA43-29E5-45A3-98BB-3EC02BFAA9E2}" dateTime="2021-02-16T17:43:00.000000000Z" userName=" " r:id="rId4" minRId="6" maxRId="7" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1947,7 +1947,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6470D23D-AEC2-469C-BB3C-9AD79530E678}" dateTime="2021-02-16T15:33:00.000000000Z" userName=" " r:id="rId5" minRId="9" maxRId="9" maxSheetId="7">
+  <header guid="{3FC0A448-3A4A-4BF4-8D13-54627C49FE52}" dateTime="2021-02-16T18:06:00.000000000Z" userName=" " r:id="rId5" minRId="8" maxRId="9" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1957,7 +1957,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{1F82C6C4-C1EC-4AFC-B63D-F555ABA4AC32}" dateTime="2021-02-16T15:35:00.000000000Z" userName=" " r:id="rId6" minRId="10" maxRId="13" maxSheetId="7">
+  <header guid="{9F2D774B-9B70-4389-9781-C316D9FC1460}" dateTime="2021-02-16T17:35:00.000000000Z" userName=" " r:id="rId6" minRId="10" maxRId="11" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1967,7 +1967,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{086878BA-B54C-4A05-B764-7333DF3F4947}" dateTime="2021-02-16T15:37:00.000000000Z" userName=" " r:id="rId7" minRId="14" maxRId="14" maxSheetId="7">
+  <header guid="{59C383AF-702B-4BF9-9872-F2B3D85B606D}" dateTime="2021-02-16T17:36:00.000000000Z" userName=" " r:id="rId7" minRId="12" maxRId="13" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1977,7 +1977,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{5F2F1F2E-156E-4366-90BF-0FEF64F74171}" dateTime="2021-02-16T17:58:00.000000000Z" userName=" " r:id="rId8" minRId="15" maxRId="15" maxSheetId="7">
+  <header guid="{36B38DB8-D06F-49D7-B44B-BA8A805C7AE1}" dateTime="2021-02-16T17:37:00.000000000Z" userName=" " r:id="rId8" minRId="14" maxRId="15" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1987,7 +1987,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6793CB85-BD3D-438E-9737-3843CA8F02BB}" dateTime="2021-02-16T17:59:00.000000000Z" userName=" " r:id="rId9" minRId="16" maxRId="16" maxSheetId="7">
+  <header guid="{C1FB7B23-2D37-4002-839F-454239728F89}" dateTime="2021-02-16T17:38:00.000000000Z" userName=" " r:id="rId9" minRId="16" maxRId="17" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1997,7 +1997,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{864066BD-D552-498C-AB9A-BA42CCE5AB55}" dateTime="2021-02-16T18:01:00.000000000Z" userName=" " r:id="rId10" minRId="17" maxRId="17" maxSheetId="7">
+  <header guid="{CDA7062A-F5D6-47EB-8DB8-AA4C96BB8366}" dateTime="2021-02-16T17:40:00.000000000Z" userName=" " r:id="rId10" minRId="18" maxRId="18" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2007,7 +2007,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{EA53141E-9217-4FC7-BB40-4B3514B4AB99}" dateTime="2021-02-16T18:03:00.000000000Z" userName=" " r:id="rId11" minRId="18" maxRId="19" maxSheetId="7">
+  <header guid="{E475256A-75A8-4750-86B7-DBA90EEAEC7C}" dateTime="2021-02-16T17:41:00.000000000Z" userName=" " r:id="rId11" minRId="19" maxRId="20" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2017,7 +2017,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{3B49C647-2B97-4009-B8AC-BAB194DE3E98}" dateTime="2021-02-16T17:43:00.000000000Z" userName=" " r:id="rId12" minRId="20" maxRId="21" maxSheetId="7">
+  <header guid="{14C524FA-10EB-4914-ACD9-DCF60C7654CA}" dateTime="2021-02-16T15:31:00.000000000Z" userName=" " r:id="rId12" minRId="21" maxRId="21" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2027,7 +2027,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{8D952353-A148-4F19-A4FA-A2C9E589729C}" dateTime="2021-02-16T18:06:00.000000000Z" userName=" " r:id="rId13" minRId="22" maxRId="23" maxSheetId="7">
+  <header guid="{FCBCE21F-9477-4D37-83A6-5585D25AA894}" dateTime="2021-02-16T17:42:00.000000000Z" userName=" " r:id="rId13" minRId="22" maxRId="22" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2037,7 +2037,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{8B0DF753-55BA-469C-8CCC-E1E607162C23}" dateTime="2021-02-16T17:35:00.000000000Z" userName=" " r:id="rId14" minRId="24" maxRId="25" maxSheetId="7">
+  <header guid="{B6F716D0-6302-4567-9505-14299D9E6746}" dateTime="2021-02-16T18:12:00.000000000Z" userName=" " r:id="rId14" minRId="23" maxRId="23" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2047,7 +2047,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{87A26D1E-006E-4ACE-9CF3-B4A975BD95D4}" dateTime="2021-02-16T17:36:00.000000000Z" userName=" " r:id="rId15" minRId="26" maxRId="27" maxSheetId="7">
+  <header guid="{1C87A8A4-F805-42B5-89B0-2D7F062526E0}" dateTime="2021-02-16T18:13:00.000000000Z" userName=" " r:id="rId15" minRId="24" maxRId="24" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2057,7 +2057,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{D19E2B6C-6352-4DB9-B42B-7A7692132797}" dateTime="2021-02-16T17:37:00.000000000Z" userName=" " r:id="rId16" minRId="28" maxRId="29" maxSheetId="7">
+  <header guid="{EBDF5975-A85A-46B0-87F0-784909943D3B}" dateTime="2021-02-16T17:44:00.000000000Z" userName=" " r:id="rId16" minRId="25" maxRId="28" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2067,7 +2067,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{52831D17-EF36-4CD9-98B3-F55952298861}" dateTime="2021-02-16T17:38:00.000000000Z" userName=" " r:id="rId17" minRId="30" maxRId="31" maxSheetId="7">
+  <header guid="{EE627949-4DFF-4174-985C-7ECB399DFE25}" dateTime="2021-02-16T18:14:00.000000000Z" userName=" " r:id="rId17" minRId="29" maxRId="29" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2077,7 +2077,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{308D37A9-A032-444F-A936-286BE24D7783}" dateTime="2021-02-16T17:40:00.000000000Z" userName=" " r:id="rId18" minRId="32" maxRId="32" maxSheetId="7">
+  <header guid="{62E79C5E-5983-4AE2-948A-E8CCE0C90589}" dateTime="2021-02-16T18:16:00.000000000Z" userName=" " r:id="rId18" minRId="30" maxRId="30" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2087,7 +2087,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{36529D9D-847D-46B0-9F49-E5F34DA3A77A}" dateTime="2021-02-16T17:41:00.000000000Z" userName=" " r:id="rId19" minRId="33" maxRId="34" maxSheetId="7">
+  <header guid="{36AF1071-140A-4EBF-9483-86BE9E92E930}" dateTime="2021-02-16T15:39:00.000000000Z" userName=" " r:id="rId19" minRId="31" maxRId="31" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2097,7 +2097,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{4DA7347C-BAF0-4036-AB05-E3FCAE601A4B}" dateTime="2021-02-16T17:42:00.000000000Z" userName=" " r:id="rId20" minRId="35" maxRId="35" maxSheetId="7">
+  <header guid="{DC82D677-2486-498D-AD94-6AFD2399AD48}" dateTime="2021-02-16T17:45:00.000000000Z" userName=" " r:id="rId20" minRId="32" maxRId="32" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2107,7 +2107,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6DDB52B4-0F7B-4DFA-B581-458C55CEA3AC}" dateTime="2021-02-16T18:12:00.000000000Z" userName=" " r:id="rId21" minRId="36" maxRId="36" maxSheetId="7">
+  <header guid="{80D4AEF0-3F17-44BE-86EE-CF9B06AA8753}" dateTime="2021-02-16T17:48:00.000000000Z" userName=" " r:id="rId21" minRId="33" maxRId="33" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2117,7 +2117,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6F908CB5-5CC2-4D31-B024-91DD3F7A2898}" dateTime="2021-02-16T18:13:00.000000000Z" userName=" " r:id="rId22" minRId="37" maxRId="37" maxSheetId="7">
+  <header guid="{E5C16DA8-EA33-41C4-BDDF-1175FEFBE334}" dateTime="2021-02-16T17:49:00.000000000Z" userName=" " r:id="rId22" minRId="34" maxRId="34" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2127,7 +2127,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{D2B1F965-C60F-4CF9-89EE-C9A4E738DF82}" dateTime="2021-02-16T17:44:00.000000000Z" userName=" " r:id="rId23" minRId="38" maxRId="41" maxSheetId="7">
+  <header guid="{A3E43740-5A66-4840-A9AC-7EAAEAA25C5C}" dateTime="2021-02-16T15:32:00.000000000Z" userName=" " r:id="rId23" minRId="35" maxRId="37" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2137,7 +2137,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{B5D70D94-E975-44DF-B752-2C8BA9AFCEE0}" dateTime="2021-02-16T18:14:00.000000000Z" userName=" " r:id="rId24" minRId="42" maxRId="42" maxSheetId="7">
+  <header guid="{FB07DDEE-CF04-4F01-901E-208C5CABF698}" dateTime="2021-02-16T15:29:00.000000000Z" userName=" " r:id="rId24" minRId="38" maxRId="38" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2147,7 +2147,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{F6821565-9363-4F63-A9BD-E99950E500EF}" dateTime="2021-02-16T18:16:00.000000000Z" userName=" " r:id="rId25" minRId="43" maxRId="43" maxSheetId="7">
+  <header guid="{AFC3A449-B2B6-40C9-BD87-69F9D64D3300}" dateTime="2021-02-16T15:30:00.000000000Z" userName=" " r:id="rId25" minRId="39" maxRId="39" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2157,7 +2157,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{52A3BFEC-31FD-41EB-A5BB-4C9660575455}" dateTime="2021-02-16T15:39:00.000000000Z" userName=" " r:id="rId26" minRId="44" maxRId="44" maxSheetId="7">
+  <header guid="{57A0152C-8867-4AE8-96D8-FEE102E91CC5}" dateTime="2021-02-17T20:37:00.000000000Z" userName=" " r:id="rId26" minRId="40" maxRId="40" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2167,7 +2167,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{26103682-AC5E-471B-A220-C9F41262E02D}" dateTime="2021-02-16T17:45:00.000000000Z" userName=" " r:id="rId27" minRId="45" maxRId="45" maxSheetId="7">
+  <header guid="{B546B22C-55F7-4E4C-B539-A8823D4C3090}" dateTime="2021-02-17T20:38:00.000000000Z" userName=" " r:id="rId27" minRId="41" maxRId="42" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2177,7 +2177,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{83AFDAAB-9244-41BB-9A46-831166069DCE}" dateTime="2021-02-16T17:48:00.000000000Z" userName=" " r:id="rId28" minRId="46" maxRId="46" maxSheetId="7">
+  <header guid="{5A6A7613-0549-4DF1-9BE2-4E45BE42B65B}" dateTime="2021-02-16T15:38:00.000000000Z" userName=" " r:id="rId28" minRId="43" maxRId="44" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2187,7 +2187,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{6D4AE0C1-77FD-40D6-A87A-00CFF4AFB4CF}" dateTime="2021-02-16T17:49:00.000000000Z" userName=" " r:id="rId29" minRId="47" maxRId="47" maxSheetId="7">
+  <header guid="{0FFBBAF0-5542-42E5-97FB-EF6FDC5DBE14}" dateTime="2021-02-16T15:33:00.000000000Z" userName=" " r:id="rId29" minRId="45" maxRId="45" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2197,7 +2197,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{53FB02C1-6BFC-4FB7-975C-FC95FFAFFA11}" dateTime="2021-02-16T15:29:00.000000000Z" userName=" " r:id="rId30" minRId="48" maxRId="48" maxSheetId="7">
+  <header guid="{7FCE079D-5D84-4378-89A1-72999F4F42CF}" dateTime="2021-02-16T15:35:00.000000000Z" userName=" " r:id="rId30" minRId="46" maxRId="49" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2207,7 +2207,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{0FA86F92-ED6E-4610-927E-F28499665025}" dateTime="2021-02-16T15:30:00.000000000Z" userName=" " r:id="rId31" minRId="49" maxRId="49" maxSheetId="7">
+  <header guid="{DA2841B0-A6A2-480E-BFC3-0BF89D59EE53}" dateTime="2021-02-16T15:37:00.000000000Z" userName=" " r:id="rId31" minRId="50" maxRId="50" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2217,7 +2217,7 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{B443AD7F-CFDE-4DE6-B03E-9119965C8268}" dateTime="2021-02-17T20:37:00.000000000Z" userName=" " r:id="rId32" minRId="50" maxRId="50" maxSheetId="7">
+  <header guid="{A95E2582-1B46-4BBC-B5A1-27528EDB908E}" dateTime="2021-02-16T17:58:00.000000000Z" userName=" " r:id="rId32" minRId="51" maxRId="51" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2227,7 +2227,17 @@
       <sheetId val="6"/>
     </sheetIdMap>
   </header>
-  <header guid="{AEBCA880-B033-488A-ABE0-0D3BF8B11912}" dateTime="2021-02-17T20:38:00.000000000Z" userName=" " r:id="rId33" minRId="51" maxRId="52" maxSheetId="7">
+  <header guid="{89E368E8-93F6-45CC-A43E-3A993D81B4BC}" dateTime="2021-02-16T17:59:00.000000000Z" userName=" " r:id="rId33" minRId="52" maxRId="52" maxSheetId="7">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FEEE1EC7-3F41-4468-B84C-3834F9955678}" dateTime="2021-02-18T10:50:00.000000000Z" userName=" " r:id="rId34" minRId="53" maxRId="53" maxSheetId="7">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2303,7 +2313,449 @@
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="17" ua="false" sId="2">
+  <rcc rId="18" ua="false" sId="2">
+    <oc r="AD97" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD97" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="19" ua="false" sId="2">
+    <oc r="AD99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="20" ua="false" sId="2">
+    <oc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="21" ua="false" sId="2">
+    <oc r="AL42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="22" ua="false" sId="2">
+    <oc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="23" ua="false" sId="2">
+    <oc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="24" ua="false" sId="2">
+    <oc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}.OperatingClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="25" ua="false" sId="2">
+    <oc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="26" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="27" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="28" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="29" ua="false" sId="2">
+    <oc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="30" ua="false" sId="2">
+    <oc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="31" ua="false" sId="2">
+    <oc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex, idx = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="3" ua="false" sId="2">
     <oc r="AD49" t="inlineStr">
       <is>
         <r>
@@ -2334,9 +2786,451 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="18" ua="false" sId="2">
+  <rcc rId="32" ua="false" sId="2">
+    <oc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="33" ua="false" sId="2">
+    <oc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="34" ua="false" sId="2">
+    <oc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="35" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i};idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="36" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}.; idx = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}.; idx = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="37" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}.; idx = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="38" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.; idx = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="39" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="40" ua="false" sId="2">
+    <oc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint.{i}; ; idx = AccessPointIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; </t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="41" ua="false" sId="2">
+    <oc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; </t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="42" ua="false" sId="2">
+    <oc r="AJ10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_del.lua Device.Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AJ10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_del.lua Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="43" ua="false" sId="2">
+    <oc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL108" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex, idx = NeighborBSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="44" ua="false" sId="2">
+    <oc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="45" ua="false" sId="2">
+    <oc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx = STAIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL71" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="4" ua="false" sId="2">
     <oc r="AD49" t="inlineStr">
       <is>
         <r>
@@ -2364,7 +3258,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="19" ua="false" sId="2">
+  <rcc rId="5" ua="false" sId="2">
     <oc r="AD52" t="inlineStr">
       <is>
         <r>
@@ -2395,9 +3289,260 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="20" ua="false" sId="2">
+  <rcc rId="46" ua="false" sId="2">
+    <oc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.; idx = OpClassScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="47" ua="false" sId="2">
+    <oc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i};idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="48" ua="false" sId="2">
+    <oc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i};idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL54" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="49" ua="false" sId="2">
+    <oc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL99" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="50" ua="false" sId="2">
+    <oc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx = ChannelScanIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL102" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="51" ua="false" sId="2">
+    <oc r="AD42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AD42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOperatingClassesIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="52" ua="false" sId="2">
+    <oc r="AL42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AL42" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOperatingClassesIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog34.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="53" ua="false" sId="2">
+    <oc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AH10" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; ; idx = AccessPointIndex</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="6" ua="false" sId="2">
     <oc r="AL30" t="inlineStr">
       <is>
         <r>
@@ -2425,7 +3570,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="21" ua="false" sId="2">
+  <rcc rId="7" ua="false" sId="2">
     <oc r="AL42" t="inlineStr">
       <is>
         <r>
@@ -2456,9 +3601,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="22" ua="false" sId="2">
+  <rcc rId="8" ua="false" sId="2">
     <oc r="AD49" t="inlineStr">
       <is>
         <r>
@@ -2486,7 +3631,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="23" ua="false" sId="2">
+  <rcc rId="9" ua="false" sId="2">
     <oc r="AD52" t="inlineStr">
       <is>
         <r>
@@ -2517,9 +3662,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="24" ua="false" sId="2">
+  <rcc rId="10" ua="false" sId="2">
     <oc r="AD30" t="inlineStr">
       <is>
         <r>
@@ -2547,7 +3692,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="25" ua="false" sId="2">
+  <rcc rId="11" ua="false" sId="2">
     <oc r="AD42" t="inlineStr">
       <is>
         <r>
@@ -2578,9 +3723,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="26" ua="false" sId="2">
+  <rcc rId="12" ua="false" sId="2">
     <oc r="AD47" t="inlineStr">
       <is>
         <r>
@@ -2608,7 +3753,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="27" ua="false" sId="2">
+  <rcc rId="13" ua="false" sId="2">
     <oc r="AD49" t="inlineStr">
       <is>
         <r>
@@ -2639,9 +3784,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="28" ua="false" sId="2">
+  <rcc rId="14" ua="false" sId="2">
     <oc r="AD52" t="inlineStr">
       <is>
         <r>
@@ -2669,7 +3814,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="29" ua="false" sId="2">
+  <rcc rId="15" ua="false" sId="2">
     <oc r="AD54" t="inlineStr">
       <is>
         <r>
@@ -2700,9 +3845,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="30" ua="false" sId="2">
+  <rcc rId="16" ua="false" sId="2">
     <oc r="AD71" t="inlineStr">
       <is>
         <r>
@@ -2730,7 +3875,7 @@
       </is>
     </nc>
   </rcc>
-  <rcc rId="31" ua="false" sId="2">
+  <rcc rId="17" ua="false" sId="2">
     <oc r="AD94" t="inlineStr">
       <is>
         <r>
@@ -2761,1118 +3906,12 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="32" ua="false" sId="2">
-    <oc r="AD97" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD97" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="33" ua="false" sId="2">
-    <oc r="AD99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,OpClassScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="34" ua="false" sId="2">
-    <oc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="3" ua="false" sId="2">
-    <oc r="AL42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="35" ua="false" sId="2">
-    <oc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Controller.Network.Device.{i}.DeviceIndex,Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="36" ua="false" sId="2">
-    <oc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="37" ua="false" sId="2">
-    <oc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD52" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.Capabilities.OperatingClass.$$.NonOperable;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}.OperatingClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="38" ua="false" sId="2">
-    <oc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="39" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="40" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="41" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="42" ua="false" sId="2">
-    <oc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="43" ua="false" sId="2">
-    <oc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.ScanResult.OpClassScan.$$.ChannelScan.$$.NeighborBSS.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex,Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex,NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="44" ua="false" sId="2">
-    <oc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex, idx = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="45" ua="false" sId="2">
-    <oc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="46" ua="false" sId="2">
-    <oc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="47" ua="false" sId="2">
-    <oc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.ChannelScanIndex, idx5 = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="4" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i};idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="5" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}.; idx = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}.; idx = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="6" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}.; idx = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="48" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.; idx = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="49" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="50" ua="false" sId="2">
-    <oc r="AH10" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint.{i}; ; idx = AccessPointIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AH10" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; </t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="51" ua="false" sId="2">
-    <oc r="AH10" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint; </t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AH10" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_add.lua Controller.Network.AccessPoint</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="52" ua="false" sId="2">
-    <oc r="AJ10" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_del.lua Device.Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AJ10" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_del.lua Controller.Network.AccessPoint.$$; AccessPointIndex;</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="7" ua="false" sId="2">
-    <oc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL108" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.NeighborBSS.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex, idx = NeighborBSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8" ua="false" sId="2">
-    <oc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="9" ua="false" sId="2">
-    <oc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx = STAIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL71" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.STA.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.BSS.{i}.BSSIndex, idx4 = STAIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="10" ua="false" sId="2">
-    <oc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.; idx = OpClassScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="11" ua="false" sId="2">
-    <oc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i};idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL49" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.Capabilities.OperatingClass.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="12" ua="false" sId="2">
-    <oc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i};idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL54" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.BSS.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = BSSIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="13" ua="false" sId="2">
-    <oc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL99" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = OpClassScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="14" ua="false" sId="2">
-    <oc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx = ChannelScanIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL102" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Device.Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.ChannelScan.{i}.; idx1 = Controller.Network.Device.{i}.DeviceIndex, idx2 = Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = Controller.Network.Device.{i}.Radio.{i}.ScanResult.OpClassScan.{i}.OpClassScanIndex, idx4 = ChannelScanIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="15" ua="false" sId="2">
-    <oc r="AD42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AD42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_get.lua Controller.Network.Device.$$.Radio.$$.CurrentOperatingClasses.$$;Device.Controller.Network.Device.{i}.DeviceIndex,Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex,CurrentOperatingClassesIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="16" ua="false" sId="2">
-    <oc r="AL42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOpClassIndex</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="AL42" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">prplmesh_getall.lua Controller.Network.Device.{i}.Radio.{i}.CurrentOperatingClasses.{i}; idx1 = Device.Controller.Network.Device.{i}.DeviceIndex, idx2 = Device.Controller.Network.Device.{i}.Radio.{i}.RadioIndex, idx3 = CurrentOperatingClassesIndex</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3973,18 +4012,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="topRight" activeCell="AF1" activeCellId="0" sqref="AF1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF17" activeCellId="0" sqref="AF17"/>
+      <selection pane="bottomRight" activeCell="AH17" activeCellId="0" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14005,7 +14044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14096,7 +14135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14366,7 +14405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14520,7 +14559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>

</xml_diff>